<commit_message>
fix UI and deploy
</commit_message>
<xml_diff>
--- a/public/sample_pond_parameters.xlsx.xlsx
+++ b/public/sample_pond_parameters.xlsx.xlsx
@@ -69,10 +69,10 @@
     <t xml:space="preserve"> mg/l</t>
   </si>
   <si>
-    <t>f7067e30-4bb1-4812-99fb-db4639e6ca04</t>
-  </si>
-  <si>
-    <t>NO</t>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>36691e1f-7c63-40ef-ad40-5e0647a8492f</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,10 +500,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>

</xml_diff>